<commit_message>
Switched Context flow chart with Testing evaluation
</commit_message>
<xml_diff>
--- a/Gantt Chart Proper.xlsx
+++ b/Gantt Chart Proper.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="1" r:id="rId1"/>
     <sheet name="TTPI" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -151,11 +151,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d&quot;/&quot;m&quot;/&quot;yy"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -430,6 +430,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -443,18 +455,6 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +479,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -624,7 +624,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FA49-495C-A3B7-D7C38E97A3F0}"/>
             </c:ext>
@@ -747,7 +747,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FA49-495C-A3B7-D7C38E97A3F0}"/>
             </c:ext>
@@ -763,11 +763,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="537970816"/>
-        <c:axId val="537967864"/>
+        <c:axId val="383491496"/>
+        <c:axId val="383486400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="537970816"/>
+        <c:axId val="383491496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +810,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537967864"/>
+        <c:crossAx val="383486400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="537967864"/>
+        <c:axId val="383486400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="43038"/>
@@ -870,7 +870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537970816"/>
+        <c:crossAx val="383491496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -948,7 +948,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -1029,7 +1029,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2603-49A0-AF6F-D533E97E9252}"/>
+            </c:ext>
             <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
               <c14:invertSolidFillFmt>
                 <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
@@ -1038,9 +1041,6 @@
                   </a:solidFill>
                 </c14:spPr>
               </c14:invertSolidFillFmt>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2603-49A0-AF6F-D533E97E9252}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1112,7 +1112,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2603-49A0-AF6F-D533E97E9252}"/>
+            </c:ext>
             <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
               <c14:invertSolidFillFmt>
                 <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
@@ -1121,9 +1124,6 @@
                   </a:solidFill>
                 </c14:spPr>
               </c14:invertSolidFillFmt>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2603-49A0-AF6F-D533E97E9252}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1136,11 +1136,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="400727009"/>
-        <c:axId val="813806857"/>
+        <c:axId val="384901952"/>
+        <c:axId val="384909008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="400727009"/>
+        <c:axId val="384901952"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1160,7 +1160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="813806857"/>
+        <c:crossAx val="384909008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1168,7 +1168,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="813806857"/>
+        <c:axId val="384909008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,7 +1202,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400727009"/>
+        <c:crossAx val="384901952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2104,20 +2104,20 @@
   <dimension ref="A1:AA40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="48.5" customWidth="1"/>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="83" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="83" customWidth="1"/>
-    <col min="6" max="6" width="13.875" customWidth="1"/>
-    <col min="7" max="7" width="11.25" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" style="78" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="78" customWidth="1"/>
+    <col min="6" max="6" width="13.8984375" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" customWidth="1"/>
     <col min="8" max="8" width="32.5" customWidth="1"/>
-    <col min="9" max="27" width="11.25" customWidth="1"/>
+    <col min="9" max="27" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1">
@@ -2130,10 +2130,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="68" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="50" t="s">
@@ -2154,10 +2154,10 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="69">
         <v>43038</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="69">
         <v>43042</v>
       </c>
       <c r="F2" s="51">
@@ -2194,10 +2194,10 @@
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="70">
         <v>43038</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E3" s="69">
         <v>43042</v>
       </c>
       <c r="F3" s="51">
@@ -2214,14 +2214,14 @@
       <c r="Q3" s="19"/>
       <c r="R3" s="20"/>
       <c r="S3" s="21"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
-      <c r="X3" s="68"/>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="80"/>
+      <c r="AA3" s="80"/>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -2233,10 +2233,10 @@
       <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="69">
         <v>43038</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="69">
         <v>43042</v>
       </c>
       <c r="F4" s="51">
@@ -2272,10 +2272,10 @@
       <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="71">
         <v>43038</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="71">
         <v>43044</v>
       </c>
       <c r="F5" s="51">
@@ -2311,10 +2311,10 @@
       <c r="C6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="72">
         <v>43038</v>
       </c>
-      <c r="E6" s="77">
+      <c r="E6" s="72">
         <v>43051</v>
       </c>
       <c r="F6" s="51">
@@ -2350,10 +2350,10 @@
       <c r="C7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="71">
         <v>43038</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="71">
         <v>43044</v>
       </c>
       <c r="F7" s="51">
@@ -2383,8 +2383,8 @@
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="49"/>
@@ -2413,12 +2413,12 @@
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="77">
+        <v>25</v>
+      </c>
+      <c r="D9" s="72">
         <v>43045</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="72">
         <v>43051</v>
       </c>
       <c r="F9" s="51">
@@ -2454,10 +2454,10 @@
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="71">
         <v>43052</v>
       </c>
-      <c r="E10" s="76">
+      <c r="E10" s="71">
         <v>43057</v>
       </c>
       <c r="F10" s="51">
@@ -2492,10 +2492,10 @@
       <c r="C11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="72">
         <v>43058</v>
       </c>
-      <c r="E11" s="77">
+      <c r="E11" s="72">
         <v>43068</v>
       </c>
       <c r="F11" s="51">
@@ -2530,10 +2530,10 @@
       <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="76">
+      <c r="D12" s="71">
         <v>43062</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="71">
         <v>43068</v>
       </c>
       <c r="F12" s="51">
@@ -2568,10 +2568,10 @@
       <c r="C13" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="79">
+      <c r="D13" s="74">
         <v>43064</v>
       </c>
-      <c r="E13" s="79">
+      <c r="E13" s="74">
         <v>43073</v>
       </c>
       <c r="F13" s="51">
@@ -2606,10 +2606,10 @@
       <c r="C14" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="75">
         <v>43073</v>
       </c>
-      <c r="E14" s="80">
+      <c r="E14" s="75">
         <v>43131</v>
       </c>
       <c r="F14" s="51">
@@ -2644,10 +2644,10 @@
       <c r="C15" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="79">
+      <c r="D15" s="74">
         <v>43045</v>
       </c>
-      <c r="E15" s="79">
+      <c r="E15" s="74">
         <v>43131</v>
       </c>
       <c r="F15" s="51">
@@ -2682,8 +2682,8 @@
       <c r="C16" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
       <c r="F16" s="16"/>
       <c r="G16" s="34"/>
       <c r="L16" s="23"/>
@@ -2707,8 +2707,8 @@
       <c r="A17" s="40"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
       <c r="L17" s="32"/>
@@ -2736,10 +2736,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
+        <v>23</v>
+      </c>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
       <c r="F18" s="39"/>
       <c r="G18" s="34"/>
       <c r="L18" s="32"/>
@@ -2769,8 +2769,8 @@
       <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="22"/>
       <c r="G19" s="34"/>
       <c r="L19" s="32"/>
@@ -2794,8 +2794,8 @@
       <c r="A20" s="39"/>
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="39"/>
       <c r="G20" s="34"/>
       <c r="L20" s="26"/>
@@ -2819,8 +2819,8 @@
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="22"/>
       <c r="G21" s="27"/>
       <c r="L21" s="26"/>
@@ -2844,8 +2844,8 @@
       <c r="A22" s="39"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="39"/>
       <c r="G22" s="27"/>
       <c r="L22" s="32"/>
@@ -2869,8 +2869,8 @@
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="22"/>
       <c r="G23" s="27"/>
       <c r="L23" s="32"/>
@@ -2894,8 +2894,8 @@
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
       <c r="F24" s="16"/>
       <c r="G24" s="27"/>
       <c r="L24" s="32"/>
@@ -2919,8 +2919,8 @@
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
       <c r="F25" s="22"/>
       <c r="G25" s="27"/>
       <c r="L25" s="32"/>
@@ -2944,8 +2944,8 @@
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="16"/>
       <c r="G26" s="27"/>
       <c r="L26" s="32"/>
@@ -2969,8 +2969,8 @@
       <c r="A27" s="43"/>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="43"/>
       <c r="G27" s="44"/>
       <c r="L27" s="21"/>
@@ -2994,8 +2994,8 @@
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
       <c r="F28" s="45"/>
       <c r="G28" s="44"/>
       <c r="L28" s="21"/>
@@ -3019,8 +3019,8 @@
       <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="22"/>
       <c r="G29" s="27"/>
       <c r="L29" s="21"/>
@@ -3029,23 +3029,23 @@
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
       <c r="Q29" s="46"/>
-      <c r="R29" s="71"/>
-      <c r="S29" s="68"/>
-      <c r="T29" s="68"/>
-      <c r="U29" s="68"/>
-      <c r="V29" s="68"/>
-      <c r="W29" s="70"/>
-      <c r="X29" s="68"/>
-      <c r="Y29" s="68"/>
-      <c r="Z29" s="68"/>
+      <c r="R29" s="83"/>
+      <c r="S29" s="80"/>
+      <c r="T29" s="80"/>
+      <c r="U29" s="80"/>
+      <c r="V29" s="80"/>
+      <c r="W29" s="82"/>
+      <c r="X29" s="80"/>
+      <c r="Y29" s="80"/>
+      <c r="Z29" s="80"/>
       <c r="AA29" s="21"/>
     </row>
     <row r="30" spans="1:27" ht="15" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="16"/>
       <c r="G30" s="27"/>
       <c r="L30" s="21"/>
@@ -3054,23 +3054,23 @@
       <c r="O30" s="21"/>
       <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
-      <c r="R30" s="67"/>
-      <c r="S30" s="68"/>
-      <c r="T30" s="68"/>
-      <c r="U30" s="68"/>
-      <c r="V30" s="68"/>
-      <c r="W30" s="67"/>
-      <c r="X30" s="68"/>
-      <c r="Y30" s="68"/>
-      <c r="Z30" s="68"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="80"/>
+      <c r="T30" s="80"/>
+      <c r="U30" s="80"/>
+      <c r="V30" s="80"/>
+      <c r="W30" s="79"/>
+      <c r="X30" s="80"/>
+      <c r="Y30" s="80"/>
+      <c r="Z30" s="80"/>
       <c r="AA30" s="21"/>
     </row>
     <row r="31" spans="1:27" ht="15" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
       <c r="F31" s="22"/>
       <c r="G31" s="27"/>
       <c r="L31" s="21"/>
@@ -3094,8 +3094,8 @@
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
       <c r="F32" s="16"/>
       <c r="G32" s="27"/>
       <c r="R32" s="21"/>
@@ -3107,8 +3107,8 @@
       <c r="A33" s="22"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
       <c r="F33" s="22"/>
       <c r="G33" s="27"/>
       <c r="H33" s="21"/>
@@ -3130,8 +3130,8 @@
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
       <c r="F34" s="16"/>
       <c r="G34" s="27"/>
       <c r="H34" s="21"/>
@@ -3172,7 +3172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="10" spans="1:6">
       <c r="B10" s="7" t="s">

</xml_diff>